<commit_message>
Updated System Design and IDD
System Design includes Client-Server API, Client, and Server, and changes were made to Requester-submitted By-Ingredient search parameters and Requester-received Matching products. Changed name and content of "From Requester" in IDD and Name in "To Requester".
</commit_message>
<xml_diff>
--- a/Interface_Design/Requester_and_Ice-Cream_System_Interface_Design.xlsx
+++ b/Interface_Design/Requester_and_Ice-Cream_System_Interface_Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Ice-Cream_Project\Interface_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4F544A-180A-4B28-A2AD-401833B99809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84F828E-3E55-48E4-88A9-AB8E0175B671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="1260" windowWidth="18960" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19270" yWindow="120" windowWidth="18960" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Created: 12/26/20 by Tom Lever</t>
   </si>
@@ -75,18 +75,12 @@
     <t>Product image</t>
   </si>
   <si>
-    <t>By-ingredient search</t>
-  </si>
-  <si>
     <t>Product image - Open</t>
   </si>
   <si>
     <t>Product image - Closed</t>
   </si>
   <si>
-    <t>List of products</t>
-  </si>
-  <si>
     <t>Products</t>
   </si>
   <si>
@@ -139,6 +133,21 @@
   </si>
   <si>
     <t>Requester and Ice-Cream System Interface Design</t>
+  </si>
+  <si>
+    <t>Matching products</t>
+  </si>
+  <si>
+    <t>By-ingredient search parameters</t>
+  </si>
+  <si>
+    <t>Chosen allergens</t>
+  </si>
+  <si>
+    <t>Chosen dietary certifications</t>
+  </si>
+  <si>
+    <t>Chosen sourcing values</t>
   </si>
 </sst>
 </file>
@@ -489,18 +498,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -527,11 +534,29 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>16</v>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -549,10 +574,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -578,7 +603,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -587,13 +612,13 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
@@ -611,19 +636,19 @@
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="4"/>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="4"/>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="4"/>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
@@ -643,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
@@ -651,7 +676,7 @@
         <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
@@ -659,7 +684,7 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
@@ -667,31 +692,31 @@
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
@@ -699,12 +724,13 @@
         <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B31:B40"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>